<commit_message>
[Resource Manager] Adjust HostInfo FreeCpu
</commit_message>
<xml_diff>
--- a/resource/hostInfo_template.xlsx
+++ b/resource/hostInfo_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="17020"/>
+    <workbookView windowHeight="13420"/>
   </bookViews>
   <sheets>
     <sheet name="Host Information" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
   <si>
     <t>Host Name</t>
   </si>
@@ -69,7 +69,7 @@
     </r>
   </si>
   <si>
-    <t>OS</t>
+    <t>OS Version</t>
   </si>
   <si>
     <t>Kernel</t>
@@ -78,7 +78,8 @@
     <t>CpuCores</t>
   </si>
   <si>
-    <t>Memory</t>
+    <t>Memory
+(GiB)</t>
   </si>
   <si>
     <t>Nic</t>
@@ -184,7 +185,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[status(optional): Available/Reserved]</t>
+      <t>[status(optional): Available/Reserved, Capacity Unit: GiB]</t>
     </r>
   </si>
   <si>
@@ -212,7 +213,7 @@
     <t>X86_64</t>
   </si>
   <si>
-    <t>CentOS</t>
+    <t>CentOS 7.0</t>
   </si>
   <si>
     <t>5.4.0</t>
@@ -230,7 +231,7 @@
     <t>SSD</t>
   </si>
   <si>
-    <t>[{"name": "vda","capacity": 256,"status": "Reserved", "path": "/", "type": "SATA"}, {"name": "vdd", "capacity": 512,"status": "Available", "path": "/mnt/vdd", "type":"SSD"}, {"name": "vde","capacity": 1024,"status": "Available","path": "/mnt/vde", "type":"SSD"}]</t>
+    <t>[{"name": "vda","capacity": 256,"status": "Reserved", "path": "/"}, {"name": "vdd", "capacity": 512,"status": "Available", "path": "/mnt/vdd"}, {"name": "vde","capacity": 1024,"status": "Available","path": "/mnt/vde"}]</t>
   </si>
   <si>
     <t>HostName2</t>
@@ -245,9 +246,6 @@
     <t>Rack2</t>
   </si>
   <si>
-    <t>Ubuntu</t>
-  </si>
-  <si>
     <t>5.2.0</t>
   </si>
   <si>
@@ -260,7 +258,7 @@
     <t>NVMeSSD</t>
   </si>
   <si>
-    <t>[{"name": "nvme0p1","capacity": 256,"status": "Reserved", "path": "/","type":"NVMeSSD"}, {"name": "nvme0p2", "capacity": 1024,"status": "Available", "path": "/mnt/path1", "type": "NVMeSSD"}, {"name": "nvme0p3","capacity": 4096,"status": "Available","path": "/mnt/path2", "type": "NVMeSSD"}]</t>
+    <t>[{"name": "nvme0p1","capacity": 256,"status": "Reserved", "path": "/"}, {"name": "nvme0p2", "capacity": 1024,"status": "Available", "path": "/mnt/path1"}, {"name": "nvme0p3","capacity": 4096,"status": "Available","path": "/mnt/path2"}]</t>
   </si>
   <si>
     <t>HostName3</t>
@@ -292,9 +290,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
@@ -330,6 +328,82 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -338,35 +412,30 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -380,94 +449,23 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -501,187 +499,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -698,32 +696,8 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
       <bottom style="medium">
         <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -733,6 +707,15 @@
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -792,90 +775,105 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -884,65 +882,65 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="17" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -956,6 +954,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1283,7 +1284,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1295,10 +1296,10 @@
     <col min="5" max="5" width="10.3303571428571" customWidth="1"/>
     <col min="6" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.0803571428571" customWidth="1"/>
-    <col min="9" max="9" width="10.4107142857143" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
     <col min="11" max="11" width="8.66071428571429" customWidth="1"/>
-    <col min="12" max="12" width="7.25" customWidth="1"/>
+    <col min="12" max="12" width="7.73214285714286" customWidth="1"/>
     <col min="14" max="14" width="17.6607142857143" customWidth="1"/>
     <col min="15" max="15" width="19.3303571428571" customWidth="1"/>
     <col min="16" max="16" width="11.5803571428571" customWidth="1"/>
@@ -1339,7 +1340,7 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="L1" s="5" t="s">
         <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
@@ -1358,7 +1359,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" ht="106" spans="1:17">
+    <row r="2" ht="88" spans="1:17">
       <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
@@ -1407,11 +1408,11 @@
       <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="6" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="3" ht="106" spans="1:17">
+    <row r="3" ht="88" spans="1:17">
       <c r="A3" s="3" t="s">
         <v>32</v>
       </c>
@@ -1437,10 +1438,10 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" t="s">
         <v>36</v>
-      </c>
-      <c r="J3" t="s">
-        <v>37</v>
       </c>
       <c r="K3">
         <v>16</v>
@@ -1452,24 +1453,24 @@
         <v>27</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="P3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="P3" s="3" t="s">
+      <c r="Q3" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="Q3" s="5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="4" ht="88" spans="1:17">
       <c r="A4" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>42</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>43</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
@@ -1481,19 +1482,19 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>45</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="I4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4" t="s">
         <v>36</v>
-      </c>
-      <c r="J4" t="s">
-        <v>37</v>
       </c>
       <c r="K4">
         <v>16</v>
@@ -1505,16 +1506,16 @@
         <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="Q4" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
[Resource Manager] Adjust import host template
</commit_message>
<xml_diff>
--- a/resource/hostInfo_template.xlsx
+++ b/resource/hostInfo_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="13420"/>
+    <workbookView windowHeight="17020"/>
   </bookViews>
   <sheets>
     <sheet name="Host Information" sheetId="1" r:id="rId1"/>
@@ -28,13 +28,13 @@
     <t>Login Password</t>
   </si>
   <si>
-    <t>Region</t>
-  </si>
-  <si>
-    <t>Zone</t>
-  </si>
-  <si>
-    <t>Rack</t>
+    <t>RegionID</t>
+  </si>
+  <si>
+    <t>ZoneID</t>
+  </si>
+  <si>
+    <t>RackID</t>
   </si>
   <si>
     <r>
@@ -69,10 +69,34 @@
     </r>
   </si>
   <si>
-    <t>OS Version</t>
-  </si>
-  <si>
-    <t>Kernel</t>
+    <r>
+      <t xml:space="preserve">OS Version
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(optional)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kernel
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(optional)</t>
+    </r>
   </si>
   <si>
     <t>CpuCores</t>
@@ -82,7 +106,19 @@
 (GiB)</t>
   </si>
   <si>
-    <t>Nic</t>
+    <r>
+      <t xml:space="preserve">Nic
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <charset val="134"/>
+      </rPr>
+      <t>(optional)</t>
+    </r>
   </si>
   <si>
     <r>
@@ -174,6 +210,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Disks
 </t>
     </r>
@@ -290,12 +333,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="27">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -334,11 +377,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -350,16 +399,100 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -373,96 +506,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
@@ -488,6 +531,14 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -505,13 +556,49 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -523,163 +610,127 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -696,8 +747,23 @@
       <left/>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -706,56 +772,6 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
@@ -777,16 +793,51 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </right>
       <top style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
       </top>
       <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -795,88 +846,88 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -888,59 +939,59 @@
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="27" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -954,6 +1005,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1284,7 +1338,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O3" sqref="O3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1297,7 +1351,7 @@
     <col min="6" max="7" width="10" customWidth="1"/>
     <col min="8" max="8" width="10.0803571428571" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
-    <col min="10" max="10" width="9" customWidth="1"/>
+    <col min="10" max="10" width="8.48214285714286" customWidth="1"/>
     <col min="11" max="11" width="8.66071428571429" customWidth="1"/>
     <col min="12" max="12" width="7.73214285714286" customWidth="1"/>
     <col min="14" max="14" width="17.6607142857143" customWidth="1"/>
@@ -1331,19 +1385,19 @@
       <c r="H1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="I1" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="J1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="L1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="5" t="s">
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
@@ -1408,7 +1462,7 @@
       <c r="P2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="Q2" s="6" t="s">
+      <c r="Q2" s="7" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1461,7 +1515,7 @@
       <c r="P3" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="Q3" s="6" t="s">
+      <c r="Q3" s="7" t="s">
         <v>40</v>
       </c>
     </row>
@@ -1514,7 +1568,7 @@
       <c r="P4" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="Q4" s="6" t="s">
+      <c r="Q4" s="7" t="s">
         <v>48</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[Resource Manager] Format host purpose and fix some issues while review
</commit_message>
<xml_diff>
--- a/resource/hostInfo_template.xlsx
+++ b/resource/hostInfo_template.xlsx
@@ -70,6 +70,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">OS Version
 </t>
     </r>
@@ -78,6 +85,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>(optional)</t>
@@ -85,6 +93,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Kernel
 </t>
     </r>
@@ -93,6 +108,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>(optional)</t>
@@ -107,6 +123,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t xml:space="preserve">Nic
 </t>
     </r>
@@ -115,6 +138,7 @@
         <b/>
         <sz val="10"/>
         <color theme="1"/>
+        <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
       <t>(optional)</t>
@@ -146,6 +170,30 @@
   </si>
   <si>
     <r>
+      <t>Component Purpose</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
+      <t>[Compute/Storage/Schedule]</t>
+    </r>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="12"/>
@@ -153,7 +201,7 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>Component Purpose</t>
+      <t>Disk Type</t>
     </r>
     <r>
       <rPr>
@@ -172,8 +220,8 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>[Compute/Storage/
-Schedule]</t>
+      <t>[NVMeSSD/
+SSD/SATA]</t>
     </r>
   </si>
   <si>
@@ -185,38 +233,6 @@
         <rFont val="宋体"/>
         <charset val="134"/>
       </rPr>
-      <t>Disk Type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t xml:space="preserve">
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
-      <t>[NVMeSSD/
-SSD/SATA]</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="宋体"/>
-        <charset val="134"/>
-      </rPr>
       <t xml:space="preserve">Disks
 </t>
     </r>
@@ -295,7 +311,7 @@
     <t>DataMigration</t>
   </si>
   <si>
-    <t>Storage</t>
+    <t>Compute,Storage</t>
   </si>
   <si>
     <t>NVMeSSD</t>
@@ -319,7 +335,7 @@
     <t>EnterpriseManager</t>
   </si>
   <si>
-    <t>Schedule</t>
+    <t>Compute,Storage,Schedule</t>
   </si>
   <si>
     <t>SATA</t>
@@ -338,7 +354,7 @@
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="26">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -371,21 +387,29 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -399,28 +423,22 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -429,46 +447,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -482,33 +463,68 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,14 +547,6 @@
       <color theme="1"/>
       <name val="宋体"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
     </font>
   </fonts>
   <fills count="33">
@@ -556,181 +564,181 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -749,21 +757,6 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -807,6 +800,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top style="thin">
@@ -827,17 +835,17 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
       </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
       </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
       </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -846,85 +854,85 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -933,61 +941,61 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1338,7 +1346,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1355,7 +1363,7 @@
     <col min="11" max="11" width="8.66071428571429" customWidth="1"/>
     <col min="12" max="12" width="7.73214285714286" customWidth="1"/>
     <col min="14" max="14" width="17.6607142857143" customWidth="1"/>
-    <col min="15" max="15" width="19.3303571428571" customWidth="1"/>
+    <col min="15" max="15" width="24.4017857142857" customWidth="1"/>
     <col min="16" max="16" width="11.5803571428571" customWidth="1"/>
     <col min="17" max="17" width="50.9107142857143" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
[Resource Manager] Adjust default RegionID and ZoneID in host template file.
</commit_message>
<xml_diff>
--- a/resource/hostInfo_template.xlsx
+++ b/resource/hostInfo_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45">
   <si>
     <t>Host Name</t>
   </si>
@@ -170,6 +170,13 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <charset val="134"/>
+      </rPr>
       <t>Component Purpose</t>
     </r>
     <r>
@@ -263,7 +270,7 @@
     <t>Region1</t>
   </si>
   <si>
-    <t>Zone1</t>
+    <t>Zone1_1</t>
   </si>
   <si>
     <t>Rack1</t>
@@ -299,12 +306,6 @@
     <t>192.168.56.12</t>
   </si>
   <si>
-    <t>Zone2</t>
-  </si>
-  <si>
-    <t>Rack2</t>
-  </si>
-  <si>
     <t>5.2.0</t>
   </si>
   <si>
@@ -324,12 +325,6 @@
   </si>
   <si>
     <t>192.168.56.13</t>
-  </si>
-  <si>
-    <t>Zone3</t>
-  </si>
-  <si>
-    <t>Rack3</t>
   </si>
   <si>
     <t>EnterpriseManager</t>
@@ -349,10 +344,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="26">
     <font>
@@ -400,18 +395,18 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <sz val="11"/>
+      <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -423,6 +418,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="18"/>
       <color theme="3"/>
@@ -431,25 +433,17 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color rgb="FFFA7D00"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -463,6 +457,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
       <name val="宋体"/>
@@ -478,9 +480,31 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FFFFFFFF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -489,35 +513,6 @@
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -570,175 +565,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -757,6 +752,15 @@
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -786,6 +790,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
@@ -796,6 +815,17 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -814,182 +844,147 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="31" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="24" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1346,7 +1341,7 @@
   <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.16071428571429" defaultRowHeight="17.6" outlineLevelRow="3"/>
@@ -1491,10 +1486,10 @@
         <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>35</v>
+        <v>23</v>
       </c>
       <c r="H3" s="3" t="s">
         <v>24</v>
@@ -1503,7 +1498,7 @@
         <v>25</v>
       </c>
       <c r="J3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K3">
         <v>16</v>
@@ -1515,24 +1510,24 @@
         <v>27</v>
       </c>
       <c r="N3" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="P3" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="O3" s="3" t="s">
+      <c r="Q3" s="7" t="s">
         <v>38</v>
-      </c>
-      <c r="P3" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q3" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="4" ht="88" spans="1:17">
       <c r="A4" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>19</v>
@@ -1544,10 +1539,10 @@
         <v>21</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>43</v>
+        <v>22</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>44</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>24</v>
@@ -1556,7 +1551,7 @@
         <v>25</v>
       </c>
       <c r="J4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K4">
         <v>16</v>
@@ -1568,16 +1563,16 @@
         <v>27</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="P4" s="3" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="Q4" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>